<commit_message>
Unnecessary scenario data are not displayed in graphs. Variable of x axis are changed to 3 gasses emissions.
</commit_message>
<xml_diff>
--- a/define/variablemap.xlsx
+++ b/define/variablemap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ochie\Documents\AsianMCSAnalysis\define\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4CF5E4-41AF-4212-B385-50302E321B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607FAF58-B8F3-4C8B-8952-B9EAA1B6EFEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9E2815BC-9F67-4991-BD26-333A0D3FFB28}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9E2815BC-9F67-4991-BD26-333A0D3FFB28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5819" uniqueCount="2330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5821" uniqueCount="2332">
   <si>
     <t>AGMIP|AGR|Area</t>
   </si>
@@ -7026,6 +7026,14 @@
   </si>
   <si>
     <t>"Yield|Sugarcrops"</t>
+  </si>
+  <si>
+    <t>"Emissions|3 Gases"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Emissions|3 Gases</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -7391,8 +7399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74550ED2-D651-4963-9FC3-D02AFA9C2514}">
   <dimension ref="A1:E1170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A1138" workbookViewId="0">
+      <selection activeCell="E1161" sqref="E1161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -23649,6 +23657,12 @@
       </c>
       <c r="B1161" t="s">
         <v>2320</v>
+      </c>
+      <c r="D1161" t="s">
+        <v>2330</v>
+      </c>
+      <c r="E1161" t="s">
+        <v>2331</v>
       </c>
     </row>
     <row r="1162" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Add graphs for absolute value of energy intensity, carbon intensity and RE share
</commit_message>
<xml_diff>
--- a/define/variablemap.xlsx
+++ b/define/variablemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ochie\Documents\AsianMCSAnalysis\define\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607FAF58-B8F3-4C8B-8952-B9EAA1B6EFEE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBFF512-4644-4D03-9B97-E4DDBBA6F7F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9E2815BC-9F67-4991-BD26-333A0D3FFB28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5821" uniqueCount="2332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5833" uniqueCount="2344">
   <si>
     <t>AGMIP|AGR|Area</t>
   </si>
@@ -7033,6 +7033,48 @@
   </si>
   <si>
     <t>Emissions|3 Gases</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Carbon Intensity(3 Gases/PE)</t>
+  </si>
+  <si>
+    <t>Energy Intensity(PE/GDP|PPP)</t>
+  </si>
+  <si>
+    <t>Share of Reneable Energy</t>
+  </si>
+  <si>
+    <t>Share of Reneable Energy|Non-Biomass</t>
+  </si>
+  <si>
+    <t>Carbon Intensity Improvement Speed(3 Gases/PE)</t>
+  </si>
+  <si>
+    <t>Energy Intensity Improvement Speed(PE/GDP|PPP)</t>
+  </si>
+  <si>
+    <t>"Carbon Intensity(3 Gases/PE)"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Energy Intensity(PE/GDP|PPP)"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Carbon Intensity Improvement Speed(3 Gases/PE)"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Energy Intensity Improvement Speed(PE/GDP|PPP)"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Share of Reneable Energy"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Share of Reneable Energy|Non-Biomass"</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -7400,7 +7442,7 @@
   <dimension ref="A1:E1170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1138" workbookViewId="0">
-      <selection activeCell="E1161" sqref="E1161"/>
+      <selection activeCell="D1163" sqref="D1163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -23672,6 +23714,12 @@
       <c r="B1162" t="s">
         <v>2321</v>
       </c>
+      <c r="D1162" t="s">
+        <v>2338</v>
+      </c>
+      <c r="E1162" t="s">
+        <v>2332</v>
+      </c>
     </row>
     <row r="1163" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1163" t="s">
@@ -23680,6 +23728,12 @@
       <c r="B1163" t="s">
         <v>2322</v>
       </c>
+      <c r="D1163" t="s">
+        <v>2339</v>
+      </c>
+      <c r="E1163" t="s">
+        <v>2333</v>
+      </c>
     </row>
     <row r="1164" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1164" t="s">
@@ -23688,6 +23742,12 @@
       <c r="B1164" t="s">
         <v>2323</v>
       </c>
+      <c r="D1164" t="s">
+        <v>2340</v>
+      </c>
+      <c r="E1164" t="s">
+        <v>2336</v>
+      </c>
     </row>
     <row r="1165" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1165" t="s">
@@ -23696,6 +23756,12 @@
       <c r="B1165" t="s">
         <v>2324</v>
       </c>
+      <c r="D1165" t="s">
+        <v>2341</v>
+      </c>
+      <c r="E1165" t="s">
+        <v>2337</v>
+      </c>
     </row>
     <row r="1166" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1166" t="s">
@@ -23704,6 +23770,12 @@
       <c r="B1166" t="s">
         <v>2325</v>
       </c>
+      <c r="D1166" t="s">
+        <v>2342</v>
+      </c>
+      <c r="E1166" t="s">
+        <v>2334</v>
+      </c>
     </row>
     <row r="1167" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1167" t="s">
@@ -23711,6 +23783,12 @@
       </c>
       <c r="B1167" t="s">
         <v>2326</v>
+      </c>
+      <c r="D1167" t="s">
+        <v>2343</v>
+      </c>
+      <c r="E1167" t="s">
+        <v>2335</v>
       </c>
     </row>
     <row r="1168" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Revise energy and carbon intensity improvement speed. Add graphs of electrification.
</commit_message>
<xml_diff>
--- a/define/variablemap.xlsx
+++ b/define/variablemap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ochie\Documents\AsianMCSAnalysis\define\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBFF512-4644-4D03-9B97-E4DDBBA6F7F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20FE9A8-ED11-4F32-805C-CB09F0CD2F1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9E2815BC-9F67-4991-BD26-333A0D3FFB28}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9E2815BC-9F67-4991-BD26-333A0D3FFB28}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5833" uniqueCount="2344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5839" uniqueCount="2350">
   <si>
     <t>AGMIP|AGR|Area</t>
   </si>
@@ -7075,6 +7075,29 @@
   </si>
   <si>
     <t>"Share of Reneable Energy|Non-Biomass"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Carbon Intensity Improvement Speed(3 Gases/PE)|vs2020"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Energy Intensity Improvement Speed(PE/GDP|PPP)|vs2020"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Carbon Intensity Improvement Speed(3 Gases/PE)|vs2020</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Energy Intensity Improvement Speed(PE/GDP|PPP)|vs2020</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Electrification Rate</t>
+  </si>
+  <si>
+    <t>"Electrification Rate"</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -7441,9 +7464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74550ED2-D651-4963-9FC3-D02AFA9C2514}">
   <dimension ref="A1:E1170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1138" workbookViewId="0">
-      <selection activeCell="D1163" sqref="D1163"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>
@@ -23771,10 +23792,10 @@
         <v>2325</v>
       </c>
       <c r="D1166" t="s">
-        <v>2342</v>
+        <v>2344</v>
       </c>
       <c r="E1166" t="s">
-        <v>2334</v>
+        <v>2346</v>
       </c>
     </row>
     <row r="1167" spans="1:5" x14ac:dyDescent="0.45">
@@ -23785,10 +23806,10 @@
         <v>2326</v>
       </c>
       <c r="D1167" t="s">
-        <v>2343</v>
+        <v>2345</v>
       </c>
       <c r="E1167" t="s">
-        <v>2335</v>
+        <v>2347</v>
       </c>
     </row>
     <row r="1168" spans="1:5" x14ac:dyDescent="0.45">
@@ -23798,21 +23819,39 @@
       <c r="B1168" t="s">
         <v>2327</v>
       </c>
-    </row>
-    <row r="1169" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="D1168" t="s">
+        <v>2342</v>
+      </c>
+      <c r="E1168" t="s">
+        <v>2334</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1169" t="s">
         <v>1167</v>
       </c>
       <c r="B1169" t="s">
         <v>2328</v>
       </c>
-    </row>
-    <row r="1170" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="D1169" t="s">
+        <v>2343</v>
+      </c>
+      <c r="E1169" t="s">
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1170" t="s">
         <v>1168</v>
       </c>
       <c r="B1170" t="s">
         <v>2329</v>
+      </c>
+      <c r="D1170" t="s">
+        <v>2349</v>
+      </c>
+      <c r="E1170" t="s">
+        <v>2348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add two indicators. Add adjusted R-squared to graphs.
</commit_message>
<xml_diff>
--- a/define/variablemap.xlsx
+++ b/define/variablemap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ochie\Documents\AsianMCSAnalysis\define\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3373DDEC-4148-45DF-9733-65370CAB5017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA80804D-EECB-4DA8-82B5-FA27F318B621}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9E2815BC-9F67-4991-BD26-333A0D3FFB28}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5843" uniqueCount="2355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5847" uniqueCount="2359">
   <si>
     <t>AGMIP|AGR|Area</t>
   </si>
@@ -7120,6 +7120,20 @@
   </si>
   <si>
     <t>c</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Additional Investment</t>
+  </si>
+  <si>
+    <t>Additional Investment per GDP</t>
+  </si>
+  <si>
+    <t>"Additional Investment"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Additional Investment per GDP"</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -7484,10 +7498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74550ED2-D651-4963-9FC3-D02AFA9C2514}">
-  <dimension ref="A1:E1172"/>
+  <dimension ref="A1:E1174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1140" workbookViewId="0">
-      <selection activeCell="D1172" sqref="D1172"/>
+    <sheetView tabSelected="1" topLeftCell="A1146" workbookViewId="0">
+      <selection activeCell="A1170" sqref="A1170:B1170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -23865,6 +23879,12 @@
       </c>
     </row>
     <row r="1170" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1170" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B1170" t="s">
+        <v>2329</v>
+      </c>
       <c r="D1170" t="s">
         <v>2352</v>
       </c>
@@ -23873,12 +23893,6 @@
       </c>
     </row>
     <row r="1171" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1171" t="s">
-        <v>1168</v>
-      </c>
-      <c r="B1171" t="s">
-        <v>2329</v>
-      </c>
       <c r="D1171" t="s">
         <v>2349</v>
       </c>
@@ -23892,6 +23906,22 @@
       </c>
       <c r="E1172" t="s">
         <v>2350</v>
+      </c>
+    </row>
+    <row r="1173" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D1173" t="s">
+        <v>2357</v>
+      </c>
+      <c r="E1173" t="s">
+        <v>2355</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="D1174" t="s">
+        <v>2358</v>
+      </c>
+      <c r="E1174" t="s">
+        <v>2356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>